<commit_message>
started update activity diagram for trip management
</commit_message>
<xml_diff>
--- a/backlog-sprints.xlsx
+++ b/backlog-sprints.xlsx
@@ -15,31 +15,35 @@
     <sheet name="system sheet" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Product Backlog'!$B$4:$H$114</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Product Backlog'!$B$4:$H$114</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Product Backlog'!$B$4:$H$114</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$114</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$114</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Product Backlog'!$B$4:$H$118</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Product Backlog'!$B$4:$H$118</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$118</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$118</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$118</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -48,42 +52,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="H3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">513334:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Report to Estimate Scrum unit the computed amount of scrum units found in Sprint sheet</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -496,7 +464,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t xml:space="preserve">Scrum Excel sheet</t>
   </si>
@@ -603,12 +571,6 @@
     <t xml:space="preserve">Based on a work at touilleur-express.fr.</t>
   </si>
   <si>
-    <t xml:space="preserve">Edited by:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last edited:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Titre</t>
   </si>
   <si>
@@ -675,7 +637,10 @@
     <t xml:space="preserve">Utilisateur</t>
   </si>
   <si>
-    <t xml:space="preserve">Gérer mon compte</t>
+    <t xml:space="preserve">Modifier mon compte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer mon compte</t>
   </si>
   <si>
     <t xml:space="preserve">Définir mon ou mes véhicules</t>
@@ -687,10 +652,16 @@
     <t xml:space="preserve">Réserver un trajet</t>
   </si>
   <si>
+    <t xml:space="preserve">Annuler une réservation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valider un trajet</t>
   </si>
   <si>
-    <t xml:space="preserve">Payer mon trajet ?</t>
+    <t xml:space="preserve">Annuler un trajet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payer mon trajet</t>
   </si>
   <si>
     <t xml:space="preserve">Voir les réservations passager sur mon trajet</t>
@@ -699,10 +670,13 @@
     <t xml:space="preserve">Accepter ou refuser les réservations sur mon trajet</t>
   </si>
   <si>
+    <t xml:space="preserve">Voir les trajets en cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste trajets</t>
+  </si>
+  <si>
     <t xml:space="preserve">Voir les trajets effectués</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Historique</t>
   </si>
   <si>
     <t xml:space="preserve">Evaluer un utilisateur avec qui j’ai partagé un trajet</t>
@@ -939,21 +913,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="16"/>
       <color rgb="FF3366FF"/>
       <name val="Avenir LT Std 35 Light"/>
@@ -1049,6 +1008,21 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1468,11 +1442,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1492,55 +1466,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="25" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="23" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="26" fillId="2" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="24" fillId="2" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="21" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="28" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="26" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1572,11 +1546,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="21" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1584,7 +1558,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1596,11 +1570,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="26" fillId="2" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="24" fillId="2" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1608,7 +1582,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="21" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1620,7 +1594,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1640,7 +1614,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1664,7 +1638,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1676,7 +1650,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1684,7 +1658,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="26" fillId="2" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="24" fillId="2" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1708,7 +1682,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1752,7 +1726,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1884,8 +1858,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.359130565583634"/>
-          <c:y val="0.0436419125127162"/>
+          <c:x val="0.35914407130232"/>
+          <c:y val="0.0436463526299725"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1897,10 +1871,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.102888086642599"/>
-          <c:y val="0.203763987792472"/>
-          <c:w val="0.721307160048135"/>
-          <c:h val="0.590233977619532"/>
+          <c:x val="0.102891955924937"/>
+          <c:y val="0.203784718689592"/>
+          <c:w val="0.721296679327592"/>
+          <c:h val="0.590192288126971"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2082,11 +2056,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="70560511"/>
-        <c:axId val="28601959"/>
+        <c:axId val="41613606"/>
+        <c:axId val="82085665"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70560511"/>
+        <c:axId val="41613606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2134,8 +2108,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.435243682310469"/>
-              <c:y val="0.885656154628688"/>
+              <c:x val="0.43526005039299"/>
+              <c:y val="0.885644521314478"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2171,14 +2145,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28601959"/>
+        <c:crossAx val="82085665"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28601959"/>
+        <c:axId val="82085665"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,8 +2200,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0301594464500602"/>
-              <c:y val="0.361546286876907"/>
+              <c:x val="0.0301981873566244"/>
+              <c:y val="0.361481330755926"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2263,7 +2237,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70560511"/>
+        <c:crossAx val="41613606"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2374,8 +2348,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.359153543307087"/>
-          <c:y val="0.0436463526299725"/>
+          <c:x val="0.359171219056056"/>
+          <c:y val="0.0436507936507936"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2387,10 +2361,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.102903543307087"/>
-          <c:y val="0.203784718689592"/>
-          <c:w val="0.721259842519685"/>
-          <c:h val="0.590294027876691"/>
+          <c:x val="0.102908607707072"/>
+          <c:y val="0.203805453805454"/>
+          <c:w val="0.721246124317142"/>
+          <c:h val="0.59025234025234"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2572,11 +2546,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="831738"/>
-        <c:axId val="78435184"/>
+        <c:axId val="54342524"/>
+        <c:axId val="34972693"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="831738"/>
+        <c:axId val="54342524"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2624,8 +2598,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.435285433070866"/>
-              <c:y val="0.885644521314478"/>
+              <c:x val="0.435306855652345"/>
+              <c:y val="0.885632885632886"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2661,14 +2635,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78435184"/>
+        <c:crossAx val="34972693"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78435184"/>
+        <c:axId val="34972693"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2716,8 +2690,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0302165354330709"/>
-              <c:y val="0.361481330755926"/>
+              <c:x val="0.0302672375609036"/>
+              <c:y val="0.361416361416361"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2753,7 +2727,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="831738"/>
+        <c:crossAx val="54342524"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2828,9 +2802,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>615960</xdr:colOff>
+      <xdr:colOff>615600</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2844,7 +2818,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533520" y="6004440"/>
-          <a:ext cx="833400" cy="297720"/>
+          <a:ext cx="833040" cy="297360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2860,10 +2834,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2874,9 +2844,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>455760</xdr:colOff>
+      <xdr:colOff>455400</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2885,7 +2855,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="640080" y="4293720"/>
-        <a:ext cx="9572760" cy="3538440"/>
+        <a:ext cx="9572400" cy="3538080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2898,7 +2868,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2909,9 +2879,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>455760</xdr:colOff>
+      <xdr:colOff>455400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>136080</xdr:rowOff>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2920,7 +2890,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="640080" y="4255920"/>
-        <a:ext cx="7314840" cy="3538080"/>
+        <a:ext cx="7314480" cy="3537720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3762,7 +3732,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
@@ -3807,51 +3777,47 @@
       <c r="A3" s="13"/>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
-      <c r="E3" s="16" t="s">
-        <v>23</v>
-      </c>
+      <c r="E3" s="16"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="18" t="s">
-        <v>24</v>
-      </c>
+      <c r="H3" s="18"/>
       <c r="I3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20"/>
       <c r="B4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="F4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="G4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="H4" s="25" t="s">
         <v>29</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>32</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>34</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
@@ -3860,13 +3826,13 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="29"/>
       <c r="C6" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
@@ -3875,13 +3841,13 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="29"/>
       <c r="C7" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
@@ -3890,13 +3856,13 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="29"/>
       <c r="C8" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
@@ -3905,13 +3871,13 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="29"/>
       <c r="C9" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>41</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
@@ -3920,13 +3886,13 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="29"/>
       <c r="C10" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
@@ -3935,13 +3901,13 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="29"/>
       <c r="C11" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
@@ -3950,13 +3916,13 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="29"/>
       <c r="C12" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
@@ -3965,13 +3931,13 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="29"/>
       <c r="C13" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>48</v>
-      </c>
       <c r="E13" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
@@ -3980,12 +3946,14 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="29"/>
       <c r="C14" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="29"/>
+        <v>47</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>34</v>
+      </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
@@ -3993,13 +3961,13 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="29"/>
       <c r="C15" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
@@ -4008,13 +3976,13 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="29"/>
       <c r="C16" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
@@ -4023,13 +3991,13 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="29"/>
       <c r="C17" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
@@ -4038,13 +4006,13 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="29"/>
       <c r="C18" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
@@ -4053,13 +4021,13 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="29"/>
       <c r="C19" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
@@ -4068,13 +4036,13 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="29"/>
       <c r="C20" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -4083,13 +4051,13 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="29"/>
       <c r="C21" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
@@ -4098,13 +4066,13 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="29"/>
       <c r="C22" s="29" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -4113,13 +4081,13 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="29"/>
       <c r="C23" s="29" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
@@ -4128,13 +4096,13 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="29"/>
       <c r="C24" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>62</v>
-      </c>
       <c r="E24" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
@@ -4142,51 +4110,110 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
+      <c r="C25" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>43</v>
+      </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
+      <c r="C26" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
       <c r="H26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="C27" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
+      <c r="C28" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:H114"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4194,8 +4221,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4227,10 +4252,10 @@
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="34" t="n">
         <v>39742</v>
@@ -4254,7 +4279,7 @@
         <v>My Product</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D2" s="34" t="n">
         <f aca="false">WORKDAY(D1,10)</f>
@@ -4287,7 +4312,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3" s="38" t="n">
         <f aca="false">D16</f>
@@ -4320,10 +4345,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
@@ -4378,16 +4403,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E6" s="44" t="n">
         <v>39650</v>
@@ -4711,7 +4736,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="73" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P16" s="37"/>
       <c r="Q16" s="37"/>
@@ -4796,7 +4821,7 @@
       <c r="B17" s="70"/>
       <c r="C17" s="37"/>
       <c r="D17" s="74" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E17" s="75" t="n">
         <f aca="false">'system sheet'!C10</f>
@@ -7389,10 +7414,10 @@
     <row r="1" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D1" s="34" t="n">
         <v>39742</v>
@@ -7415,7 +7440,7 @@
         <v>My Product</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D2" s="34" t="n">
         <f aca="false">WORKDAY(D1,10)</f>
@@ -7448,7 +7473,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3" s="38" t="n">
         <f aca="false">D17</f>
@@ -7481,10 +7506,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
@@ -7539,16 +7564,16 @@
     </row>
     <row r="6" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E6" s="44" t="n">
         <v>39650</v>
@@ -7662,7 +7687,7 @@
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="86"/>
       <c r="B7" s="48" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="50" t="n">
@@ -7886,7 +7911,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="88" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="37"/>
@@ -7971,7 +7996,7 @@
       <c r="B18" s="70"/>
       <c r="C18" s="37"/>
       <c r="D18" s="74" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E18" s="75" t="n">
         <f aca="false">'system sheet'!C11</f>
@@ -8134,7 +8159,7 @@
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="90" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="90"/>
       <c r="D2" s="90"/>
@@ -8152,27 +8177,27 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="92" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D5" s="92" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F5" s="92" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G5" s="92" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H5" s="92" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="93" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B6" s="93"/>
       <c r="C6" s="94" t="n">
@@ -8188,7 +8213,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C7" s="97" t="n">
         <v>0</v>
@@ -8214,10 +8239,10 @@
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="99" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B9" s="100" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C9" s="101" t="n">
         <v>0</v>
@@ -8250,13 +8275,13 @@
         <v>9</v>
       </c>
       <c r="N9" s="103" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="99"/>
       <c r="B10" s="104" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C10" s="105" t="n">
         <f aca="false">FORECAST(C$9, $C$6:$C$7,$N$10:$N$11)</f>
@@ -8305,7 +8330,7 @@
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="99"/>
       <c r="B11" s="104" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C11" s="105" t="n">
         <f aca="false">FORECAST(C$9, $D$6:$D$7,$N$10:$N$11)</f>
@@ -8354,7 +8379,7 @@
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="99"/>
       <c r="B12" s="104" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C12" s="105"/>
       <c r="D12" s="105"/>
@@ -8373,7 +8398,7 @@
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="99"/>
       <c r="B13" s="104" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C13" s="105"/>
       <c r="D13" s="105"/>
@@ -8389,7 +8414,7 @@
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="99"/>
       <c r="B14" s="104" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C14" s="105"/>
       <c r="D14" s="105"/>
@@ -8405,7 +8430,7 @@
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="99"/>
       <c r="B15" s="104" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C15" s="105"/>
       <c r="D15" s="105"/>
@@ -8532,12 +8557,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>